<commit_message>
added search bar + update db
</commit_message>
<xml_diff>
--- a/players.xlsx
+++ b/players.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petrm\Documents\Python\data_scout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2645969-9079-4AD0-9AF8-7EFB5DAB4F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A88F508-81A7-4EA0-81C6-B8EE19173D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{74451770-FF53-415F-8FE2-EAFB6BA6C97A}"/>
   </bookViews>
@@ -7218,9 +7218,6 @@
     <t>https://www.sofascore.com/api/v1/player/1563529/unique-tournament/41/season/70853/statistics/overall</t>
   </si>
   <si>
-    <t>Samuel</t>
-  </si>
-  <si>
     <t>Samuel Friday</t>
   </si>
   <si>
@@ -7591,6 +7588,9 @@
   </si>
   <si>
     <t>https://www.sofascore.com/cs/football/player/resley-kessels/2030419</t>
+  </si>
+  <si>
+    <t>James</t>
   </si>
 </sst>
 </file>
@@ -7987,8 +7987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8716247E-1F35-4206-BB80-F74D5865F4AF}">
   <dimension ref="A1:J366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="F232" sqref="F232"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="C349" sqref="C349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10615,7 +10615,7 @@
         <v>385</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>1428</v>
@@ -18602,25 +18602,25 @@
         <v>2390</v>
       </c>
       <c r="C348" t="s">
-        <v>2391</v>
+        <v>2514</v>
       </c>
       <c r="D348" t="s">
         <v>187</v>
       </c>
       <c r="F348" s="2" t="s">
+        <v>2391</v>
+      </c>
+      <c r="G348" s="2" t="s">
         <v>2392</v>
       </c>
-      <c r="G348" s="2" t="s">
+      <c r="H348" s="2" t="s">
         <v>2393</v>
       </c>
-      <c r="H348" s="2" t="s">
+      <c r="I348" s="2" t="s">
         <v>2394</v>
       </c>
-      <c r="I348" s="2" t="s">
+      <c r="J348" s="2" t="s">
         <v>2395</v>
-      </c>
-      <c r="J348" s="2" t="s">
-        <v>2396</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.3">
@@ -18631,7 +18631,7 @@
         <v>648</v>
       </c>
       <c r="C349" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="D349" t="s">
         <v>64</v>
@@ -18640,19 +18640,19 @@
         <v>38</v>
       </c>
       <c r="F349" s="2" t="s">
+        <v>2397</v>
+      </c>
+      <c r="G349" s="2" t="s">
         <v>2398</v>
       </c>
-      <c r="G349" s="2" t="s">
+      <c r="H349" s="2" t="s">
         <v>2399</v>
       </c>
-      <c r="H349" s="2" t="s">
+      <c r="I349" s="2" t="s">
         <v>2400</v>
       </c>
-      <c r="I349" s="2" t="s">
+      <c r="J349" s="2" t="s">
         <v>2401</v>
-      </c>
-      <c r="J349" s="2" t="s">
-        <v>2402</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.3">
@@ -18660,28 +18660,28 @@
         <v>349</v>
       </c>
       <c r="B350" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C350" t="s">
         <v>2403</v>
-      </c>
-      <c r="C350" t="s">
-        <v>2404</v>
       </c>
       <c r="D350" t="s">
         <v>64</v>
       </c>
       <c r="F350" s="2" t="s">
+        <v>2404</v>
+      </c>
+      <c r="G350" s="2" t="s">
         <v>2405</v>
       </c>
-      <c r="G350" s="2" t="s">
+      <c r="H350" s="2" t="s">
         <v>2406</v>
       </c>
-      <c r="H350" s="2" t="s">
+      <c r="I350" s="2" t="s">
         <v>2407</v>
       </c>
-      <c r="I350" s="2" t="s">
+      <c r="J350" s="2" t="s">
         <v>2408</v>
-      </c>
-      <c r="J350" s="2" t="s">
-        <v>2409</v>
       </c>
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.3">
@@ -18689,28 +18689,28 @@
         <v>350</v>
       </c>
       <c r="B351" t="s">
+        <v>2409</v>
+      </c>
+      <c r="C351" t="s">
         <v>2410</v>
-      </c>
-      <c r="C351" t="s">
-        <v>2411</v>
       </c>
       <c r="D351" t="s">
         <v>95</v>
       </c>
       <c r="F351" s="2" t="s">
+        <v>2411</v>
+      </c>
+      <c r="G351" s="2" t="s">
         <v>2412</v>
       </c>
-      <c r="G351" s="2" t="s">
+      <c r="H351" s="2" t="s">
+        <v>2414</v>
+      </c>
+      <c r="I351" s="2" t="s">
         <v>2413</v>
       </c>
-      <c r="H351" s="2" t="s">
+      <c r="J351" s="2" t="s">
         <v>2415</v>
-      </c>
-      <c r="I351" s="2" t="s">
-        <v>2414</v>
-      </c>
-      <c r="J351" s="2" t="s">
-        <v>2416</v>
       </c>
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.3">
@@ -18718,28 +18718,28 @@
         <v>351</v>
       </c>
       <c r="B352" t="s">
+        <v>2416</v>
+      </c>
+      <c r="C352" t="s">
         <v>2417</v>
-      </c>
-      <c r="C352" t="s">
-        <v>2418</v>
       </c>
       <c r="D352" t="s">
         <v>44</v>
       </c>
       <c r="F352" s="2" t="s">
+        <v>2418</v>
+      </c>
+      <c r="G352" s="2" t="s">
         <v>2419</v>
       </c>
-      <c r="G352" s="2" t="s">
+      <c r="H352" s="2" t="s">
         <v>2420</v>
       </c>
-      <c r="H352" s="2" t="s">
+      <c r="I352" s="2" t="s">
         <v>2421</v>
       </c>
-      <c r="I352" s="2" t="s">
+      <c r="J352" s="2" t="s">
         <v>2422</v>
-      </c>
-      <c r="J352" s="2" t="s">
-        <v>2423</v>
       </c>
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.3">
@@ -18750,7 +18750,7 @@
         <v>585</v>
       </c>
       <c r="C353" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="D353" t="s">
         <v>69</v>
@@ -18759,19 +18759,19 @@
         <v>8</v>
       </c>
       <c r="F353" s="2" t="s">
+        <v>2424</v>
+      </c>
+      <c r="G353" s="2" t="s">
         <v>2425</v>
       </c>
-      <c r="G353" s="2" t="s">
+      <c r="H353" s="2" t="s">
         <v>2426</v>
       </c>
-      <c r="H353" s="2" t="s">
+      <c r="I353" s="2" t="s">
         <v>2427</v>
       </c>
-      <c r="I353" s="2" t="s">
+      <c r="J353" s="2" t="s">
         <v>2428</v>
-      </c>
-      <c r="J353" s="2" t="s">
-        <v>2429</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.3">
@@ -18782,25 +18782,25 @@
         <v>607</v>
       </c>
       <c r="C354" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="D354" t="s">
         <v>64</v>
       </c>
       <c r="F354" s="2" t="s">
+        <v>2430</v>
+      </c>
+      <c r="G354" s="2" t="s">
         <v>2431</v>
       </c>
-      <c r="G354" s="2" t="s">
+      <c r="H354" s="2" t="s">
         <v>2432</v>
       </c>
-      <c r="H354" s="2" t="s">
+      <c r="I354" s="2" t="s">
         <v>2433</v>
       </c>
-      <c r="I354" s="2" t="s">
+      <c r="J354" s="2" t="s">
         <v>2434</v>
-      </c>
-      <c r="J354" s="2" t="s">
-        <v>2435</v>
       </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.3">
@@ -18808,10 +18808,10 @@
         <v>354</v>
       </c>
       <c r="B355" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="C355" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="D355" t="s">
         <v>44</v>
@@ -18820,19 +18820,19 @@
         <v>8</v>
       </c>
       <c r="F355" s="2" t="s">
+        <v>2437</v>
+      </c>
+      <c r="G355" s="2" t="s">
         <v>2438</v>
       </c>
-      <c r="G355" s="2" t="s">
+      <c r="H355" s="2" t="s">
         <v>2439</v>
       </c>
-      <c r="H355" s="2" t="s">
+      <c r="I355" s="2" t="s">
         <v>2440</v>
       </c>
-      <c r="I355" s="2" t="s">
+      <c r="J355" s="2" t="s">
         <v>2441</v>
-      </c>
-      <c r="J355" s="2" t="s">
-        <v>2442</v>
       </c>
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.3">
@@ -18843,25 +18843,25 @@
         <v>700</v>
       </c>
       <c r="C356" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="D356" t="s">
         <v>95</v>
       </c>
       <c r="F356" s="2" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G356" s="2" t="s">
         <v>2444</v>
       </c>
-      <c r="G356" s="2" t="s">
+      <c r="H356" s="2" t="s">
         <v>2445</v>
       </c>
-      <c r="H356" s="2" t="s">
+      <c r="I356" s="2" t="s">
         <v>2446</v>
       </c>
-      <c r="I356" s="2" t="s">
+      <c r="J356" s="2" t="s">
         <v>2447</v>
-      </c>
-      <c r="J356" s="2" t="s">
-        <v>2448</v>
       </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.3">
@@ -18869,28 +18869,28 @@
         <v>356</v>
       </c>
       <c r="B357" t="s">
+        <v>2448</v>
+      </c>
+      <c r="C357" t="s">
         <v>2449</v>
-      </c>
-      <c r="C357" t="s">
-        <v>2450</v>
       </c>
       <c r="D357" t="s">
         <v>187</v>
       </c>
       <c r="F357" s="2" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G357" s="2" t="s">
         <v>2451</v>
       </c>
-      <c r="G357" s="2" t="s">
+      <c r="H357" s="2" t="s">
         <v>2452</v>
       </c>
-      <c r="H357" s="2" t="s">
+      <c r="I357" s="2" t="s">
         <v>2453</v>
       </c>
-      <c r="I357" s="2" t="s">
+      <c r="J357" s="2" t="s">
         <v>2454</v>
-      </c>
-      <c r="J357" s="2" t="s">
-        <v>2455</v>
       </c>
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.3">
@@ -18901,7 +18901,7 @@
         <v>660</v>
       </c>
       <c r="C358" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="D358" t="s">
         <v>49</v>
@@ -18910,19 +18910,19 @@
         <v>38</v>
       </c>
       <c r="F358" s="2" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G358" s="2" t="s">
         <v>2457</v>
       </c>
-      <c r="G358" s="2" t="s">
+      <c r="H358" s="2" t="s">
         <v>2458</v>
       </c>
-      <c r="H358" s="2" t="s">
+      <c r="I358" s="2" t="s">
         <v>2459</v>
       </c>
-      <c r="I358" s="2" t="s">
+      <c r="J358" s="2" t="s">
         <v>2460</v>
-      </c>
-      <c r="J358" s="2" t="s">
-        <v>2461</v>
       </c>
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.3">
@@ -18933,25 +18933,25 @@
         <v>247</v>
       </c>
       <c r="C359" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="D359" t="s">
         <v>64</v>
       </c>
       <c r="F359" s="2" t="s">
+        <v>2462</v>
+      </c>
+      <c r="G359" s="2" t="s">
         <v>2463</v>
       </c>
-      <c r="G359" s="2" t="s">
+      <c r="H359" s="2" t="s">
         <v>2464</v>
       </c>
-      <c r="H359" s="2" t="s">
+      <c r="I359" s="2" t="s">
         <v>2465</v>
       </c>
-      <c r="I359" s="2" t="s">
+      <c r="J359" s="2" t="s">
         <v>2466</v>
-      </c>
-      <c r="J359" s="2" t="s">
-        <v>2467</v>
       </c>
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.3">
@@ -18959,10 +18959,10 @@
         <v>359</v>
       </c>
       <c r="B360" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C360" t="s">
         <v>2468</v>
-      </c>
-      <c r="C360" t="s">
-        <v>2469</v>
       </c>
       <c r="D360" t="s">
         <v>38</v>
@@ -18971,19 +18971,19 @@
         <v>64</v>
       </c>
       <c r="F360" s="2" t="s">
+        <v>2469</v>
+      </c>
+      <c r="G360" s="2" t="s">
         <v>2470</v>
       </c>
-      <c r="G360" s="2" t="s">
+      <c r="H360" s="2" t="s">
         <v>2471</v>
       </c>
-      <c r="H360" s="2" t="s">
+      <c r="I360" s="2" t="s">
         <v>2472</v>
       </c>
-      <c r="I360" s="2" t="s">
+      <c r="J360" s="2" t="s">
         <v>2473</v>
-      </c>
-      <c r="J360" s="2" t="s">
-        <v>2474</v>
       </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.3">
@@ -18994,25 +18994,25 @@
         <v>1192</v>
       </c>
       <c r="C361" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="D361" t="s">
         <v>49</v>
       </c>
       <c r="F361" s="2" t="s">
+        <v>2475</v>
+      </c>
+      <c r="G361" s="2" t="s">
         <v>2476</v>
       </c>
-      <c r="G361" s="2" t="s">
+      <c r="H361" s="2" t="s">
         <v>2477</v>
       </c>
-      <c r="H361" s="2" t="s">
+      <c r="I361" s="2" t="s">
         <v>2478</v>
       </c>
-      <c r="I361" s="2" t="s">
+      <c r="J361" s="2" t="s">
         <v>2479</v>
-      </c>
-      <c r="J361" s="2" t="s">
-        <v>2480</v>
       </c>
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.3">
@@ -19020,28 +19020,28 @@
         <v>361</v>
       </c>
       <c r="B362" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C362" t="s">
         <v>2481</v>
-      </c>
-      <c r="C362" t="s">
-        <v>2482</v>
       </c>
       <c r="D362" t="s">
         <v>187</v>
       </c>
       <c r="F362" s="2" t="s">
+        <v>2482</v>
+      </c>
+      <c r="G362" s="2" t="s">
         <v>2483</v>
       </c>
-      <c r="G362" s="2" t="s">
+      <c r="H362" s="2" t="s">
         <v>2484</v>
       </c>
-      <c r="H362" s="2" t="s">
+      <c r="I362" s="2" t="s">
         <v>2485</v>
       </c>
-      <c r="I362" s="2" t="s">
+      <c r="J362" s="2" t="s">
         <v>2486</v>
-      </c>
-      <c r="J362" s="2" t="s">
-        <v>2487</v>
       </c>
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.3">
@@ -19049,10 +19049,10 @@
         <v>362</v>
       </c>
       <c r="B363" t="s">
+        <v>2487</v>
+      </c>
+      <c r="C363" t="s">
         <v>2488</v>
-      </c>
-      <c r="C363" t="s">
-        <v>2489</v>
       </c>
       <c r="D363" t="s">
         <v>38</v>
@@ -19061,19 +19061,19 @@
         <v>64</v>
       </c>
       <c r="F363" s="2" t="s">
+        <v>2489</v>
+      </c>
+      <c r="G363" s="2" t="s">
         <v>2490</v>
       </c>
-      <c r="G363" s="2" t="s">
+      <c r="H363" s="2" t="s">
         <v>2491</v>
       </c>
-      <c r="H363" s="2" t="s">
+      <c r="I363" s="2" t="s">
         <v>2492</v>
       </c>
-      <c r="I363" s="2" t="s">
+      <c r="J363" s="2" t="s">
         <v>2493</v>
-      </c>
-      <c r="J363" s="2" t="s">
-        <v>2494</v>
       </c>
     </row>
     <row r="364" spans="1:10" x14ac:dyDescent="0.3">
@@ -19081,28 +19081,28 @@
         <v>363</v>
       </c>
       <c r="B364" t="s">
+        <v>2494</v>
+      </c>
+      <c r="C364" t="s">
         <v>2495</v>
-      </c>
-      <c r="C364" t="s">
-        <v>2496</v>
       </c>
       <c r="D364" t="s">
         <v>15</v>
       </c>
       <c r="F364" s="2" t="s">
+        <v>2496</v>
+      </c>
+      <c r="G364" s="2" t="s">
         <v>2497</v>
       </c>
-      <c r="G364" s="2" t="s">
+      <c r="H364" s="2" t="s">
         <v>2498</v>
       </c>
-      <c r="H364" s="2" t="s">
+      <c r="I364" s="2" t="s">
         <v>2499</v>
       </c>
-      <c r="I364" s="2" t="s">
+      <c r="J364" s="2" t="s">
         <v>2500</v>
-      </c>
-      <c r="J364" s="2" t="s">
-        <v>2501</v>
       </c>
     </row>
     <row r="365" spans="1:10" x14ac:dyDescent="0.3">
@@ -19119,19 +19119,19 @@
         <v>64</v>
       </c>
       <c r="F365" s="2" t="s">
+        <v>2501</v>
+      </c>
+      <c r="G365" s="2" t="s">
         <v>2502</v>
       </c>
-      <c r="G365" s="2" t="s">
+      <c r="H365" s="2" t="s">
         <v>2503</v>
       </c>
-      <c r="H365" s="2" t="s">
+      <c r="I365" s="2" t="s">
         <v>2504</v>
       </c>
-      <c r="I365" s="2" t="s">
+      <c r="J365" s="2" t="s">
         <v>2505</v>
-      </c>
-      <c r="J365" s="2" t="s">
-        <v>2506</v>
       </c>
     </row>
     <row r="366" spans="1:10" x14ac:dyDescent="0.3">
@@ -19139,28 +19139,28 @@
         <v>365</v>
       </c>
       <c r="B366" t="s">
+        <v>2506</v>
+      </c>
+      <c r="C366" t="s">
         <v>2507</v>
-      </c>
-      <c r="C366" t="s">
-        <v>2508</v>
       </c>
       <c r="D366" t="s">
         <v>187</v>
       </c>
       <c r="F366" s="2" t="s">
+        <v>2508</v>
+      </c>
+      <c r="G366" s="2" t="s">
         <v>2509</v>
       </c>
-      <c r="G366" s="2" t="s">
+      <c r="H366" s="2" t="s">
         <v>2510</v>
       </c>
-      <c r="H366" s="2" t="s">
+      <c r="I366" s="2" t="s">
         <v>2511</v>
       </c>
-      <c r="I366" s="2" t="s">
+      <c r="J366" s="2" t="s">
         <v>2512</v>
-      </c>
-      <c r="J366" s="2" t="s">
-        <v>2513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>